<commit_message>
use registry to keep track of workbook processes - distinguish between workbook chidren using `Registry.match/3`
</commit_message>
<xml_diff>
--- a/priv/test_workbook.xlsx
+++ b/priv/test_workbook.xlsx
@@ -11,6 +11,10 @@
     <sheet name="AnotherSheet" sheetId="2" r:id="rId2"/>
     <sheet name="sheet with space" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="test_range">FirstSheet!$A$1:$F$3</definedName>
+    <definedName name="test_range2">AnotherSheet!$A$2:$D$3</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +43,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -163,11 +167,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -451,19 +455,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="90.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="90.75" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,15 +493,23 @@
       <c r="G1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="11">
+      <c r="H1" s="10">
         <f ca="1">TODAY()</f>
-        <v>42760</v>
-      </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" ht="90.75" x14ac:dyDescent="0.3">
+        <v>42763</v>
+      </c>
+      <c r="I1" t="str">
+        <f>AnotherSheet!A1</f>
+        <v>some data</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="N1">
+        <f xml:space="preserve"> B1+C1+E1*4</f>
+        <v>1.1004</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="90.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -521,12 +534,20 @@
       <c r="G2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="10">
         <f ca="1">TODAY() -1</f>
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="90.75" x14ac:dyDescent="0.3">
+        <v>42762</v>
+      </c>
+      <c r="I2" t="str">
+        <f>AnotherSheet!A2</f>
+        <v>some data</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:N7" si="1" xml:space="preserve"> B2+C2+E2*4</f>
+        <v>2.2008000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="90.75" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -551,12 +572,20 @@
       <c r="G3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <f ca="1">TODAY() - 5</f>
-        <v>42755</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>42758</v>
+      </c>
+      <c r="I3" t="str">
+        <f>AnotherSheet!A3</f>
+        <v>some data</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="1"/>
+        <v>3.3011999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -578,12 +607,20 @@
 with
 breaks,0.0004</v>
       </c>
-      <c r="H4" s="11">
-        <f t="shared" ref="H2:H6" ca="1" si="1">TODAY()</f>
-        <v>42760</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="H4" s="10">
+        <f t="shared" ref="H4:H6" ca="1" si="2">TODAY()</f>
+        <v>42763</v>
+      </c>
+      <c r="I4" t="str">
+        <f>AnotherSheet!A4</f>
+        <v>some data</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>4.4016000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -605,12 +642,20 @@
 with
 breaks,0.0005</v>
       </c>
-      <c r="H5" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>42760</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="H5" s="10">
+        <f t="shared" ca="1" si="2"/>
+        <v>42763</v>
+      </c>
+      <c r="I5" t="str">
+        <f>AnotherSheet!A5</f>
+        <v>some data</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>5.5019999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -632,12 +677,16 @@
 with
 breaks,0.0006</v>
       </c>
-      <c r="H6" s="12">
-        <f t="shared" ca="1" si="1"/>
-        <v>42760</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="H6" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>42763</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>6.6023999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -659,8 +708,12 @@
 with
 breaks,0.0007</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>7.7027999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -683,7 +736,7 @@
 breaks,0.0008</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -706,7 +759,7 @@
 breaks,0.0009</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -729,7 +782,7 @@
 breaks,0.001</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -752,7 +805,7 @@
 breaks,0.0011</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -775,7 +828,7 @@
 breaks,0.0012</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -798,7 +851,7 @@
 breaks,0.0013</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -821,7 +874,7 @@
 breaks,0.0014</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -844,7 +897,7 @@
 breaks,0.0015</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1425,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E13"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>